<commit_message>
v1.0 test results updated
</commit_message>
<xml_diff>
--- a/pcb/v1.0/Project Outputs for Autoinformer/Autoinformer_v1.0_Tests.xlsx
+++ b/pcb/v1.0/Project Outputs for Autoinformer/Autoinformer_v1.0_Tests.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Проверяемая часть</t>
   </si>
@@ -115,9 +115,6 @@
   </si>
   <si>
     <t>Между MOUT и С31 поставить регулятор громкости (переменный резистор 10к - 47к)</t>
-  </si>
-  <si>
-    <t>Перенести сигнал на ADC2 (?)</t>
   </si>
   <si>
     <r>
@@ -191,9 +188,6 @@
     </r>
   </si>
   <si>
-    <t>Добавить кнопку для включения модуля (?)</t>
-  </si>
-  <si>
     <t>GPIO_79 не доступен в ОС</t>
   </si>
   <si>
@@ -203,14 +197,6 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>1. При остутствии внешнего питания образующийся делитель R64 | (R33 + R34) нарушает работу инвертора VT5, в результате через VT6 (открыт) напряжение аккумулятора оказывается на 3V8_EXT, ломая логику схемы.
-2. При переходе с внешнего питания на резервное напряжение аккумулятора с VT7(D) оказывается на открытом VT6 (RST не успевает сброситься и через VT5 закрыть VT6), что приводит снова к попаданию 3V8_INT на 3V8_EXT, нарушая логику схемы.</t>
-  </si>
-  <si>
-    <t>1. Изменить номиналы R64 1k, R33 22k, R34 15k или поставить ключ (или взять сигнал на делитель до инвертора (пин 1 MCP130). R63 будет избыточен. Вместо него будут R33, 34)
-2. Запитывать D6 не 3V8_EXT, а 5V . Поменять пороговое напряжение сброса</t>
-  </si>
-  <si>
     <t>Переход на аккум. питание BAK_ON GPIO</t>
   </si>
   <si>
@@ -221,18 +207,184 @@
   </si>
   <si>
     <t>Зарядка до 4.2 В макс ток 1 А</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> При остутствии внешнего питания образующийся делитель R64 | (R33 + R34) нарушает работу инвертора VT5, в результате через VT6 (открыт) напряжение аккумулятора оказывается на 3V8_EXT, ломая логику схемы.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> При переходе с внешнего питания на резервное напряжение аккумулятора с VT7(D) оказывается на открытом VT6 (RST не успевает сброситься и через VT5 закрыть VT6), что приводит снова к попаданию 3V8_INT на 3V8_EXT, нарушая логику схемы.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Если в момент зарядки аккумулятора (DA3 синий светодиод горит) происходит отключени основого питания, видимо через микросхему напряжение с батареи попадает на линию 5 V, нарушая правила питания платы.</t>
+    </r>
+  </si>
+  <si>
+    <t>Добавить кнопку для включения модуля (?) или предусмотреть цепь автосброса</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>1.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Изменить номиналы R64 1k, R33 22k, R34 15k или поставить ключ (или взять сигнал на делитель до инвертора (пин 1 MCP130). R63 будет избыточен. Вместо него будут R33, 34)
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Запитывать D6 не 3V8_EXT, а 5V . 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Поменять пороговое напряжение сброса D6  (поставить MCP130T-450I/TT) чтобы VT6 закрывался и не давал устанавливаться 3V8_EXT -&gt; 5V. </t>
+    </r>
+  </si>
+  <si>
+    <t>Перенести сигнал на ADC2 (?) или использовать встроенный в модуль монитор напряжения питания через АТ-команду</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Экран немного моргает. У i2c преобразователя диспеля необходимо отпаять подтягивающие SDA и SCL резисторы 4.7k т.к. они уже есть на плате </t>
+  </si>
+  <si>
+    <t>Заключение:</t>
+  </si>
+  <si>
+    <t>Плата пригодна для демонстрации функционала и разработки ПО, но для выхода в свет требуются доработки</t>
+  </si>
+  <si>
+    <t>Добавить конденсатор и дроссель от ЭМП по питанию.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -278,7 +430,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -301,14 +453,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -317,20 +495,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -605,7 +798,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -613,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:D34"/>
+  <dimension ref="A2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -624,7 +817,7 @@
     <col min="1" max="1" width="24.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" customWidth="1"/>
     <col min="3" max="3" width="67" customWidth="1"/>
-    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="4" max="4" width="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="30.75" customHeight="1">
@@ -641,7 +834,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" ht="30">
       <c r="A3" s="3" t="s">
         <v>20</v>
       </c>
@@ -651,8 +844,8 @@
       <c r="C3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>35</v>
+      <c r="D3" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -693,7 +886,7 @@
         <v>10</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1"/>
     </row>
@@ -787,29 +980,35 @@
         <v>10</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D16" s="1"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" ht="45">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="1"/>
+      <c r="B17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="8"/>
@@ -835,7 +1034,7 @@
         <v>10</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D20" s="1"/>
     </row>
@@ -853,32 +1052,32 @@
       <c r="C22" s="10"/>
       <c r="D22" s="9"/>
     </row>
-    <row r="23" spans="1:4" ht="120">
+    <row r="23" spans="1:4" ht="180">
       <c r="A23" s="3" t="s">
         <v>26</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="30">
+        <v>36</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="45">
       <c r="A24" s="4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>32</v>
+        <v>44</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -889,60 +1088,26 @@
         <v>10</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D25" s="1"/>
     </row>
-    <row r="27" spans="1:4">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
+    <row r="28" spans="1:4" ht="30" customHeight="1">
+      <c r="A28" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="13"/>
+      <c r="C28" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="15"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <mergeCells count="2">
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="C28:D28"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup paperSize="9" scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
i2c level shifters workaround, MOUT todo added
</commit_message>
<xml_diff>
--- a/pcb/v1.0/Project Outputs for Autoinformer/Autoinformer_v1.0_Tests.xlsx
+++ b/pcb/v1.0/Project Outputs for Autoinformer/Autoinformer_v1.0_Tests.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProjects\SocSys\auto_informer\autoinformer\pcb\v1.0\Project Outputs for Autoinformer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E12DD8CF-F2FE-447A-A513-E8B913505F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50F0F4D-ABBA-45C3-9A1D-5BCD4774A7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10110" yWindow="1830" windowWidth="17820" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7215" yWindow="240" windowWidth="17820" windowHeight="14325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>Проверяемая часть</t>
   </si>
@@ -373,6 +373,11 @@
   <si>
     <t>1. Добавить конденсатор и дроссель от ЭМП по питанию.
 2. Заменить D3 на TXS0104EPW</t>
+  </si>
+  <si>
+    <t>кротковременное КЗ на входе - ОК
+Запуск от аккума - ОК
+На входе 7 В \ 30 В - ОК</t>
   </si>
 </sst>
 </file>
@@ -816,8 +821,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:D28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,12 +1051,14 @@
       </c>
       <c r="D20" s="1"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>25</v>
       </c>
       <c r="B21" s="1"/>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>49</v>
+      </c>
       <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>